<commit_message>
Update Non-GMHO entities mapped to LSRs.xlsx
"LSR 3" identifier added to relevant classes
</commit_message>
<xml_diff>
--- a/Non-GMHO entities mapped to LSRs/Non-GMHO entities mapped to LSRs.xlsx
+++ b/Non-GMHO entities mapped to LSRs/Non-GMHO entities mapped to LSRs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/zcjtpms_ucl_ac_uk/Documents/Galenos Project/Github preparation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/zcjtpms_ucl_ac_uk/Documents/Documents/GitHub/mental-health-ontology/Non-GMHO entities mapped to LSRs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="125" documentId="8_{CDA3D274-DE34-4B6A-9AEF-88D861C7C9EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E3DEF8B-6E44-41C6-8D2D-E642D71157CB}"/>
+  <xr:revisionPtr revIDLastSave="127" documentId="8_{CDA3D274-DE34-4B6A-9AEF-88D861C7C9EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{77129073-1E78-485E-9C89-8E078210B5E4}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-15" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
   <si>
     <t>ID</t>
   </si>
@@ -166,6 +166,9 @@
   </si>
   <si>
     <t>Published</t>
+  </si>
+  <si>
+    <t>LSR 3</t>
   </si>
 </sst>
 </file>
@@ -222,7 +225,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -239,59 +242,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -613,7 +568,7 @@
   <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="P3" sqref="P3:P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -737,7 +692,9 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
+      <c r="P2" s="6" t="s">
+        <v>44</v>
+      </c>
       <c r="Q2" s="1" t="s">
         <v>42</v>
       </c>
@@ -775,7 +732,9 @@
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
+      <c r="P3" s="6" t="s">
+        <v>44</v>
+      </c>
       <c r="Q3" s="1" t="s">
         <v>42</v>
       </c>
@@ -787,43 +746,45 @@
       <c r="U3" s="6"/>
       <c r="V3" s="6"/>
     </row>
-    <row r="4" spans="1:22" s="10" customFormat="1" ht="145" x14ac:dyDescent="0.35">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:22" ht="145" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8" t="s">
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6" t="s">
+        <v>44</v>
+      </c>
       <c r="Q4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="R4" s="11"/>
+      <c r="R4" s="6"/>
       <c r="S4" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="T4" s="11"/>
-      <c r="U4" s="11"/>
-      <c r="V4" s="11"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="6"/>
     </row>
     <row r="5" spans="1:22" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
@@ -851,7 +812,9 @@
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
+      <c r="P5" s="6" t="s">
+        <v>44</v>
+      </c>
       <c r="Q5" s="1" t="s">
         <v>42</v>
       </c>
@@ -864,11 +827,11 @@
       <c r="V5" s="6"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A2:A5">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A5">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>